<commit_message>
frozen_noise and chuckrats_updated both work, also summarize_allrats
</commit_message>
<xml_diff>
--- a/docs/chuck_rats.xlsx
+++ b/docs/chuck_rats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorge/Dropbox (MIT)/research/brodylab/logistic_regression/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{088CD498-BB5F-0B46-8AB4-0CA5A0184337}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6E4E1B-F697-744D-A38C-4BDA164B3EE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13060" yWindow="460" windowWidth="15360" windowHeight="17040" xr2:uid="{32A741AC-850B-884D-B8A8-81F4BDB1D2D0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="17540" xr2:uid="{32A741AC-850B-884D-B8A8-81F4BDB1D2D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="151">
   <si>
     <t>K200</t>
   </si>
@@ -482,7 +482,10 @@
     <t>RatID</t>
   </si>
   <si>
-    <t>Used</t>
+    <t>Given by Chuck</t>
+  </si>
+  <si>
+    <t>Acquired from Server</t>
   </si>
 </sst>
 </file>
@@ -859,93 +862,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC486B4F-C458-424C-B359-682655E62672}">
-  <dimension ref="A1:B149"/>
+  <dimension ref="A1:C149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="A113" sqref="A113"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>148</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1110,497 +1120,523 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C63" s="2"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>78</v>
       </c>
       <c r="B80" s="2"/>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C80" s="2"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>79</v>
       </c>
       <c r="B81" s="2"/>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C81" s="2"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>80</v>
       </c>
       <c r="B82" s="2"/>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C82" s="2"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>84</v>
       </c>
       <c r="B86" s="2"/>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C86" s="2"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>85</v>
       </c>
       <c r="B87" s="2"/>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>87</v>
       </c>
       <c r="B89" s="2"/>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>88</v>
       </c>
       <c r="B90" s="2"/>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>90</v>
       </c>
       <c r="B92" s="2"/>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>91</v>
       </c>
       <c r="B93" s="2"/>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C93" s="2"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>93</v>
       </c>
       <c r="B95" s="2"/>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>96</v>
       </c>
       <c r="B98" s="2"/>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>99</v>
       </c>
       <c r="B101" s="2"/>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>100</v>
       </c>
       <c r="B102" s="2"/>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>101</v>
       </c>
       <c r="B103" s="2"/>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C106" s="2"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C107" s="2"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>107</v>
       </c>
       <c r="B109" s="2"/>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C109" s="2"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C110" s="2"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C112" s="2"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C115" s="2"/>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C118" s="2"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C119" s="2"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C120" s="2"/>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C124" s="2"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C125" s="2"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C126" s="2"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C127" s="2"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C128" s="2"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C131" s="2"/>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C132" s="2"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C134" s="2"/>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C135" s="2"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C136" s="2"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C137" s="2"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>142</v>
       </c>

</xml_diff>

<commit_message>
repo status at lab meeting
</commit_message>
<xml_diff>
--- a/docs/chuck_rats.xlsx
+++ b/docs/chuck_rats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorge/Dropbox (MIT)/research/brodylab/logistic_regression/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6E4E1B-F697-744D-A38C-4BDA164B3EE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47011364-65A2-A54D-8C7D-BD6AB6C1A401}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="17540" xr2:uid="{32A741AC-850B-884D-B8A8-81F4BDB1D2D0}"/>
+    <workbookView minimized="1" xWindow="28800" yWindow="-7140" windowWidth="20480" windowHeight="25140" xr2:uid="{32A741AC-850B-884D-B8A8-81F4BDB1D2D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="160">
   <si>
     <t>K200</t>
   </si>
@@ -486,13 +486,40 @@
   </si>
   <si>
     <t>Acquired from Server</t>
+  </si>
+  <si>
+    <t>Use in Analysis</t>
+  </si>
+  <si>
+    <t>Has 114,256 trials - went through freq &amp; classic, and 40 &amp; 20. Should split up. Q: Does the logit model perform better on certain tasks?</t>
+  </si>
+  <si>
+    <t>Seems like weak performer, though</t>
+  </si>
+  <si>
+    <t>40 Hz frequency rat, chuck tried two different base_freq pairs.</t>
+  </si>
+  <si>
+    <t>Frequency rat, did 40 &amp; 20 hz, two diff base_freq pairs. Frozen_noise is 20hz</t>
+  </si>
+  <si>
+    <t>40 Hz frequency rat, chuck tried two diff base_freq pairs</t>
+  </si>
+  <si>
+    <t>Classic 40</t>
+  </si>
+  <si>
+    <t>Not enough trials!</t>
+  </si>
+  <si>
+    <t>Could have more trials - 10,578. Interesting example of rat whose L bias grows as trial progresses.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -516,8 +543,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -527,6 +561,23 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -539,16 +590,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -862,100 +932,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC486B4F-C458-424C-B359-682655E62672}">
-  <dimension ref="A1:C149"/>
+  <dimension ref="A1:E149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D151" sqref="D151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1120,523 +1194,665 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>61</v>
       </c>
-      <c r="C63" s="2"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C63" s="4"/>
+      <c r="D63" s="6"/>
+      <c r="E63" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>78</v>
       </c>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B80" s="4"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>79</v>
       </c>
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>80</v>
       </c>
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>84</v>
       </c>
-      <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>85</v>
       </c>
-      <c r="B87" s="2"/>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B87" s="4"/>
+      <c r="D87" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>87</v>
       </c>
-      <c r="B89" s="2"/>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B89" s="4"/>
+      <c r="D89" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>88</v>
       </c>
-      <c r="B90" s="2"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B90" s="4"/>
+      <c r="D90" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>90</v>
       </c>
-      <c r="B92" s="2"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B92" s="4"/>
+      <c r="D92" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>91</v>
       </c>
-      <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="5">
+        <v>2</v>
+      </c>
+      <c r="E93" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>93</v>
       </c>
-      <c r="B95" s="2"/>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B95" s="4"/>
+      <c r="D95" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>96</v>
       </c>
-      <c r="B98" s="2"/>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B98" s="4"/>
+      <c r="D98" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>99</v>
       </c>
-      <c r="B101" s="2"/>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B101" s="4"/>
+      <c r="D101" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>100</v>
       </c>
-      <c r="B102" s="2"/>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B102" s="4"/>
+      <c r="D102" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>101</v>
       </c>
-      <c r="B103" s="2"/>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B103" s="4"/>
+      <c r="D103" s="5">
+        <v>1</v>
+      </c>
+      <c r="E103" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>104</v>
       </c>
-      <c r="C106" s="2"/>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C106" s="4"/>
+      <c r="D106" s="6"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>105</v>
       </c>
-      <c r="C107" s="2"/>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C107" s="4"/>
+      <c r="D107" s="5">
+        <v>1</v>
+      </c>
+      <c r="E107" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>107</v>
       </c>
-      <c r="B109" s="2"/>
-      <c r="C109" s="2"/>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B109" s="4"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="4">
+        <v>2</v>
+      </c>
+      <c r="E109" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>108</v>
       </c>
-      <c r="C110" s="2"/>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C110" s="4"/>
+      <c r="D110" s="5">
+        <v>2</v>
+      </c>
+      <c r="E110" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>110</v>
       </c>
-      <c r="C112" s="2"/>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C112" s="4"/>
+      <c r="D112" s="5">
+        <v>2</v>
+      </c>
+      <c r="E112" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C113" s="4"/>
+      <c r="D113" s="4">
+        <v>2</v>
+      </c>
+      <c r="E113" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>113</v>
       </c>
-      <c r="C115" s="2"/>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C115" s="4"/>
+      <c r="D115" s="5">
+        <v>2</v>
+      </c>
+      <c r="E115" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>116</v>
       </c>
-      <c r="C118" s="2"/>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C118" s="4"/>
+      <c r="D118" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>117</v>
       </c>
-      <c r="C119" s="2"/>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C119" s="4"/>
+      <c r="D119" s="6"/>
+      <c r="E119" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>118</v>
       </c>
-      <c r="C120" s="2"/>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C120" s="4"/>
+      <c r="D120" s="6"/>
+      <c r="E120" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>122</v>
       </c>
-      <c r="C124" s="2"/>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C124" s="4"/>
+      <c r="D124" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>123</v>
       </c>
-      <c r="C125" s="2"/>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C125" s="4"/>
+      <c r="D125" s="6"/>
+      <c r="E125" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>124</v>
       </c>
-      <c r="C126" s="2"/>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C126" s="4"/>
+      <c r="D126" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>125</v>
       </c>
-      <c r="C127" s="2"/>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C127" s="4"/>
+      <c r="D127" s="5">
+        <v>2</v>
+      </c>
+      <c r="E127" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>126</v>
       </c>
-      <c r="C128" s="2"/>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C128" s="4"/>
+      <c r="D128" s="7"/>
+      <c r="E128" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>129</v>
       </c>
-      <c r="C131" s="2"/>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C131" s="4"/>
+      <c r="D131" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>130</v>
       </c>
-      <c r="C132" s="2"/>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C132" s="4"/>
+      <c r="D132" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>132</v>
       </c>
-      <c r="C134" s="2"/>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C134" s="4"/>
+      <c r="D134" s="7"/>
+      <c r="E134" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>133</v>
       </c>
-      <c r="C135" s="2"/>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C135" s="4"/>
+      <c r="D135" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>134</v>
       </c>
-      <c r="C136" s="2"/>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C136" s="4"/>
+      <c r="D136" s="7"/>
+      <c r="E136" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>135</v>
       </c>
-      <c r="C137" s="2"/>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C137" s="4"/>
+      <c r="D137" s="7"/>
+      <c r="E137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>142</v>
       </c>

</xml_diff>